<commit_message>
Commit 25.3: Prepared Cheatsheet for PyTest,POM,Hybrid FRMWK,Selenium
</commit_message>
<xml_diff>
--- a/Selenium with Python/SeleniumDemo/Selenium Basics/CheatSheet-SeleniumPython.xlsx
+++ b/Selenium with Python/SeleniumDemo/Selenium Basics/CheatSheet-SeleniumPython.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/939c1bf4b082bbe3/Desktop/Projects/Testing Projects/Python-Pytest-Robot/Automation-Testing-with-Python/Selenium with Python/SeleniumDemo/Selenium Basics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B446F88D-CCF3-4DB6-AA5B-B6A9F6F7BFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{B446F88D-CCF3-4DB6-AA5B-B6A9F6F7BFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD5250AE-6C9C-49CC-83A3-715321387EA0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FB147EA-548A-49CC-AAE9-187A6E48BFCB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4FB147EA-548A-49CC-AAE9-187A6E48BFCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PyTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="136">
   <si>
     <t>Topic</t>
   </si>
@@ -271,16 +272,10 @@
     <t>Window Handle</t>
   </si>
   <si>
-    <t>python main_window = driver.current_window_handle</t>
-  </si>
-  <si>
     <t>Store the main window handle to switch between windows later.</t>
   </si>
   <si>
     <t>Switch to Another Window</t>
-  </si>
-  <si>
-    <t>python driver.switch_to.window(window_handle)</t>
   </si>
   <si>
     <t>Switch to a specific window using its handle.</t>
@@ -390,12 +385,329 @@
  driver.switch_to.frame("frame_name")
  driver.switch_to.default_content() # Switch back to main page</t>
   </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Snippets/Methods</t>
+  </si>
+  <si>
+    <t>Browser Setup</t>
+  </si>
+  <si>
+    <t>Initialize, navigate, maximize, and close the browser.</t>
+  </si>
+  <si>
+    <t>Form Handling</t>
+  </si>
+  <si>
+    <t>Fill text fields, submit buttons, and clear text fields.</t>
+  </si>
+  <si>
+    <t>Handle dropdowns.</t>
+  </si>
+  <si>
+    <t>Handle checkboxes and radio buttons.</t>
+  </si>
+  <si>
+    <t>find_element(By.ID, "file-upload").send_keys("file_path")</t>
+  </si>
+  <si>
+    <t>Upload files.</t>
+  </si>
+  <si>
+    <t>find_element(By.ID, "date").send_keys("YYYY-MM-DD")</t>
+  </si>
+  <si>
+    <t>Input dates.</t>
+  </si>
+  <si>
+    <t>Frame Handling</t>
+  </si>
+  <si>
+    <t>Switch to a frame or back to the main content.</t>
+  </si>
+  <si>
+    <t>Mouse Actions</t>
+  </si>
+  <si>
+    <t>Perform hover, right-click, and drag-and-drop actions.</t>
+  </si>
+  <si>
+    <t>Sorting Elements</t>
+  </si>
+  <si>
+    <t>Locate and sort table rows or elements.</t>
+  </si>
+  <si>
+    <t>Window Handling</t>
+  </si>
+  <si>
+    <t>Handle multiple browser windows.</t>
+  </si>
+  <si>
+    <t>End-to-End Testing</t>
+  </si>
+  <si>
+    <t>Perform actions for search, add to cart, and checkout.</t>
+  </si>
+  <si>
+    <t>General Waits</t>
+  </si>
+  <si>
+    <t>WebDriverWait(browser, 10).until(EC.presence_of_element_located((By.ID, "element")))</t>
+  </si>
+  <si>
+    <t>Wait for elements dynamically.</t>
+  </si>
+  <si>
+    <t>main_window = driver.current_window_handle</t>
+  </si>
+  <si>
+    <t>driver.switch_to.window(window_handle)</t>
+  </si>
+  <si>
+    <r>
+      <t>webdriver.Chrome()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>browser.get(url)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>browser.maximize_window()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>browser.quit()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>find_element(By.ID, "checkbox").click()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>find_element(By.ID, "radio").click()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ActionChains(browser).move_to_element(element).perform()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>ActionChains(browser).context_click(element).perform()
+ActionChains(browser).drag_and_drop(source, destination).perform()</t>
+    </r>
+  </si>
+  <si>
+    <t>find_element(By.ID, "username").send_keys("value")
+find_element(By.NAME, "email").send_keys("value")
+find_element(By.XPATH, "//button[text()='Submit']").click()
+find_element(By.CSS_SELECTOR, "input[type='text']").clear()</t>
+  </si>
+  <si>
+    <t>Select(browser.find_element(By.ID, "dropdown")).select_by_visible_text("Option")
+Select(browser.find_element(By.ID, "dropdown")).select_by_index(1)
+Select(browser.find_element(By.ID, "dropdown")).select_by_value("value")</t>
+  </si>
+  <si>
+    <r>
+      <t>browser.switch_to.frame("frameName")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>browser.switch_to.default_content()</t>
+    </r>
+  </si>
+  <si>
+    <t>browser.find_elements(By.XPATH, "//table/tbody/tr")
+sorted(rows, key=lambda row: row.text)</t>
+  </si>
+  <si>
+    <r>
+      <t>browser.current_window_handle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>browser.switch_to.window(handle)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>browser.close()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>find_element(By.CSS_SELECTOR, "input.search-keyword")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>find_element(By.XPATH, "//button[text()='ADD TO CART']")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>find_element(By.CSS_SELECTOR, "a.cart-icon").click()</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,6 +727,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -452,9 +771,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -469,6 +787,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -784,395 +1112,551 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F72024C-CF4B-44C4-9F5C-C8820034E78B}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="84.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.140625" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="63.75">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:4" ht="63.75">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="76.5">
+      <c r="A19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="63.75">
+      <c r="A30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="76.5">
-      <c r="A19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="6" t="s">
+      <c r="C30" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="38.25">
+      <c r="A31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="76.5">
+      <c r="A32" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="63.75">
-      <c r="A30" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B30" s="6" t="s">
+      <c r="C32" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" spans="1:3" s="9" customFormat="1">
+      <c r="A36" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="38.25">
-      <c r="A31" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" s="6" t="s">
+      <c r="B36" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="76.5">
-      <c r="A32" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>96</v>
+      <c r="C36" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="72.75">
+      <c r="A37" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="51">
+      <c r="A38" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="38.25">
+      <c r="A39" s="7"/>
+      <c r="B39" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="27.75">
+      <c r="A40" s="7"/>
+      <c r="B40" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="7"/>
+      <c r="B41" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="7"/>
+      <c r="B42" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="27.75">
+      <c r="A43" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="40.5">
+      <c r="A44" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="25.5">
+      <c r="A45" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="42.75">
+      <c r="A46" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="42.75">
+      <c r="A47" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A302B973-B305-4B5D-A03A-B2FA98A5D1BC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>